<commit_message>
apache basic user guide, until ssl(ssl is not complete)
</commit_message>
<xml_diff>
--- a/apacheDS/ldap_study.xlsx
+++ b/apacheDS/ldap_study.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="135" windowWidth="23715" windowHeight="9600" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="165" windowWidth="23715" windowHeight="9570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -692,6 +692,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>150496</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>170379</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="图片 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2057400" y="171450"/>
+          <a:ext cx="15238096" cy="8571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>380267</xdr:colOff>
+      <xdr:row>102</xdr:row>
+      <xdr:rowOff>132327</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="图片 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2057400" y="9429750"/>
+          <a:ext cx="5866667" cy="8190477"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,8 +1064,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G146"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1636,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1699,11 +1780,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C55" workbookViewId="0">
+      <selection activeCell="P64" sqref="P64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>